<commit_message>
Add new demo files.
</commit_message>
<xml_diff>
--- a/test-files/demo-files/21-genes_31-edges_Schade-data_estimation_output.xlsx
+++ b/test-files/demo-files/21-genes_31-edges_Schade-data_estimation_output.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="26715" windowHeight="14565" firstSheet="6" activeTab="12"/>
@@ -178,8 +178,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +216,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -294,6 +299,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -328,6 +334,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -503,28 +510,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -592,7 +599,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -639,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>-4.5031549633143472E-2</v>
+        <v>-2.3514515608917513E-2</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -660,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -719,16 +726,16 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>-0.18820887875915027</v>
+        <v>-4.2985429780012276E-3</v>
       </c>
       <c r="U3">
-        <v>-0.65095528818924187</v>
+        <v>-0.38624552336188939</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -751,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.61206654708051067</v>
+        <v>0.39937697108766507</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -778,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0.15615434905189041</v>
+        <v>-3.542421905660554E-2</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -796,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -831,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>7.7845882338061265E-2</v>
+        <v>0.15412923517892946</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -864,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -893,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>-1.2320858786117657</v>
+        <v>-0.56427459214233033</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -932,12 +939,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.93929482644727347</v>
+        <v>0.5757567365376377</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -982,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>-2.9706773606578425</v>
+        <v>-2.4842397030421965</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1000,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1029,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1.013078893117209</v>
+        <v>0.82087439304454191</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1056,19 +1063,19 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1.4282638085007962</v>
+        <v>1.1327684770336084</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0.54468150571223883</v>
+        <v>5.9553955918487389E-2</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1094,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1.2340986634476752</v>
+        <v>0.83975564758623178</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1133,10 +1140,10 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>-0.185164874102172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>-0.14286868649613396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>-0.88904909468606708</v>
+        <v>-0.69096132225449591</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1204,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1233,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>-0.40302862152830743</v>
+        <v>-0.22265277936169836</v>
       </c>
       <c r="K11">
-        <v>-0.89655567768121591</v>
+        <v>-0.8996511802531113</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1272,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>-1.0194851212470761E-2</v>
+        <v>6.1917390514168039E-3</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1340,12 +1347,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13">
-        <v>-0.92778950125443505</v>
+        <v>-0.73244365573264869</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1384,10 +1391,10 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>-0.43150437543692094</v>
+        <v>-0.15618188320482398</v>
       </c>
       <c r="P13">
-        <v>-0.50707438551092265</v>
+        <v>-0.42315373918803745</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1405,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>0.57442464534242077</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <v>0.5420485402062647</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1.4998823249016862</v>
+        <v>1.1928081309101652</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1476,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>-1.3615135448898985</v>
+        <v>-1.0326913096587651</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -1541,18 +1548,18 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <v>-0.40819045291287759</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <v>-0.1323464725248332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16">
-        <v>-0.53122367215985489</v>
+        <v>-0.41636565981609769</v>
       </c>
       <c r="C16">
-        <v>-0.12925221861874403</v>
+        <v>-7.6164083342736888E-2</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1570,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.62145042255406946</v>
+        <v>0.52856732884138802</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1582,16 +1589,16 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>-0.75033136906382225</v>
+        <v>-0.63500590553074698</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1.4592250590864119E-2</v>
+        <v>7.5648134719757384E-2</v>
       </c>
       <c r="P16">
-        <v>-0.30267311122041535</v>
+        <v>-0.14781774867848457</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1612,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1680,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1748,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1816,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1884,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1952,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2026,16 +2033,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2046,7 +2053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2057,7 +2064,7 @@
         <v>0.86375907025127707</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2068,7 +2075,7 @@
         <v>-8.4512094623483261E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2079,7 +2086,7 @@
         <v>-2.7036238635246637E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2090,7 +2097,7 @@
         <v>0.31799160987778807</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2101,7 +2108,7 @@
         <v>2.0785480271819798</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2112,7 +2119,7 @@
         <v>0.30848217294835073</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2123,7 +2130,7 @@
         <v>0.59772497124282109</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2134,7 +2141,7 @@
         <v>0.91436086323291665</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2145,7 +2152,7 @@
         <v>-8.3565942702706703E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2156,7 +2163,7 @@
         <v>-0.18435844242715063</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2167,7 +2174,7 @@
         <v>-0.19668331979958451</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2178,7 +2185,7 @@
         <v>-1.8473389582098459E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2189,7 +2196,7 @@
         <v>-1.0934878631044176</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>1.5145734224690381</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2211,7 +2218,7 @@
         <v>0.35275459473035098</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2222,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2233,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2244,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2255,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2266,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2283,16 +2290,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -2360,7 +2367,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2428,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2564,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2632,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2700,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2768,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2836,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2904,7 +2911,7 @@
         <v>-0.185164874102172</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2972,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3040,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3108,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3176,7 +3183,7 @@
         <v>0.57442464534242077</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3244,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3312,7 +3319,7 @@
         <v>-0.40819045291287759</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3380,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3448,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3516,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3584,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3652,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3720,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3794,16 +3801,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3823,7 +3830,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3843,7 +3850,7 @@
         <v>0.70113230605848431</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3863,7 +3870,7 @@
         <v>0.64255017478057119</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3883,7 +3890,7 @@
         <v>0.27838685574573035</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3903,7 +3910,7 @@
         <v>0.63214516421357758</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3923,7 +3930,7 @@
         <v>0.42823496437234221</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3943,7 +3950,7 @@
         <v>4.8795433799243088E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3963,7 +3970,7 @@
         <v>0.49603588739778276</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3983,7 +3990,7 @@
         <v>0.87095586318119766</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4003,7 +4010,7 @@
         <v>0.32190956976908647</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4023,7 +4030,7 @@
         <v>0.61484906015845053</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4043,7 +4050,7 @@
         <v>0.55944943488351928</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4063,7 +4070,7 @@
         <v>0.60909208857869224</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>0.18767426433518369</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4103,7 +4110,7 @@
         <v>1.0858535453491927</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -4123,7 +4130,7 @@
         <v>0.31773877344830698</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4143,7 +4150,7 @@
         <v>0.55774523004671794</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4163,7 +4170,7 @@
         <v>1.28722744723447</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4183,7 +4190,7 @@
         <v>0.83003274855249065</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4203,7 +4210,7 @@
         <v>0.29430825608901451</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -4223,7 +4230,7 @@
         <v>0.14488756926375135</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -4249,40 +4256,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4322,7 +4329,7 @@
         <v>0.48435089511121021</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4342,7 +4349,7 @@
         <v>-0.81793317594908443</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4362,7 +4369,7 @@
         <v>-0.75147912525362393</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4382,7 +4389,7 @@
         <v>0.8561782188284095</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4402,7 +4409,7 @@
         <v>-0.37427042872419891</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4422,7 +4429,7 @@
         <v>4.7013326873905102E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4442,7 +4449,7 @@
         <v>1.1248372482258766</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4462,7 +4469,7 @@
         <v>-0.30259736113703295</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4482,7 +4489,7 @@
         <v>0.55135867455041376</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4502,7 +4509,7 @@
         <v>5.8441255712988402E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4522,7 +4529,7 @@
         <v>0.34910882026688672</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4542,7 +4549,7 @@
         <v>-0.21167047056013749</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4562,7 +4569,7 @@
         <v>0.70320378879765943</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4582,7 +4589,7 @@
         <v>1.3499275795365722</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -4602,7 +4609,7 @@
         <v>0.28201661662499822</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4622,7 +4629,7 @@
         <v>-1.2538405721454773</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4642,7 +4649,7 @@
         <v>-0.34874733011964443</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -4662,7 +4669,7 @@
         <v>-0.35846845614647627</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4682,7 +4689,7 @@
         <v>0.58491872133390754</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -4702,7 +4709,7 @@
         <v>0.10759743563684412</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -4728,16 +4735,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4784,7 +4791,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4831,7 +4838,7 @@
         <v>0.35772751462172414</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4878,7 +4885,7 @@
         <v>-0.7828780372145302</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4925,7 +4932,7 @@
         <v>-0.74533690915468354</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4972,7 +4979,7 @@
         <v>0.70619458831911108</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5019,7 +5026,7 @@
         <v>-0.5028596007403463</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5066,7 +5073,7 @@
         <v>2.947576173232247E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5113,7 +5120,7 @@
         <v>1.0555313724217021</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5160,7 +5167,7 @@
         <v>-0.29154062712550571</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -5207,7 +5214,7 @@
         <v>0.77771527152471331</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -5254,7 +5261,7 @@
         <v>5.5864663129260972E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -5301,7 +5308,7 @@
         <v>0.35345576386562971</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -5348,7 +5355,7 @@
         <v>-0.19122675163066438</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5395,7 +5402,7 @@
         <v>0.75451629384667473</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -5442,7 +5449,7 @@
         <v>1.2262620760693883</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -5489,7 +5496,7 @@
         <v>0.33022485869868545</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -5536,7 +5543,7 @@
         <v>-0.64617261382469604</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -5583,7 +5590,7 @@
         <v>-0.28284669362590764</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5630,7 +5637,7 @@
         <v>-0.27370939103373881</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -5677,7 +5684,7 @@
         <v>0.51404648371380757</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -5724,7 +5731,7 @@
         <v>0.39396571986694728</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -5777,16 +5784,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5797,7 +5804,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5808,7 +5815,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5819,7 +5826,7 @@
         <v>2.5672117798516494E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -5830,7 +5837,7 @@
         <v>1.7328679513998631E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5841,7 +5848,7 @@
         <v>1.1002336199364211E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5852,7 +5859,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5863,7 +5870,7 @@
         <v>7.7016353395549478E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5874,7 +5881,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5885,7 +5892,7 @@
         <v>6.9314718055994526E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -5896,7 +5903,7 @@
         <v>1.6503504299046318E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -5907,7 +5914,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -5918,7 +5925,7 @@
         <v>5.7762265046662105E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -5929,7 +5936,7 @@
         <v>1.332975347230664E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5940,7 +5947,7 @@
         <v>1.2602676010180823E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -5951,7 +5958,7 @@
         <v>3.0136833937388925E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -5962,7 +5969,7 @@
         <v>3.3007008598092635E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -5973,7 +5980,7 @@
         <v>0.34657359027997264</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -5984,7 +5991,7 @@
         <v>0.23104906018664842</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5995,7 +6002,7 @@
         <v>2.7179999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -6006,7 +6013,7 @@
         <v>7.453195489891885E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -6017,7 +6024,7 @@
         <v>4.9510512897138946E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -6034,16 +6041,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6054,7 +6061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6065,7 +6072,7 @@
         <v>6.242669444439939E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6076,7 +6083,7 @@
         <v>0.10522676713463036</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -6087,7 +6094,7 @@
         <v>2.0858239697015505E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6098,7 +6105,7 @@
         <v>3.3546638513152101E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6109,7 +6116,7 @@
         <v>3.9619455373539288E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -6120,7 +6127,7 @@
         <v>0.18601110490312825</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -6131,7 +6138,7 @@
         <v>0.13123236983890324</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6142,7 +6149,7 @@
         <v>0.20777488757745535</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -6153,7 +6160,7 @@
         <v>5.4767494999982819E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -6164,7 +6171,7 @@
         <v>0.17120461804021761</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -6175,7 +6182,7 @@
         <v>0.13383936151722145</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -6186,7 +6193,7 @@
         <v>4.6082765886743558E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -6197,7 +6204,7 @@
         <v>0.6910371803648</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -6208,7 +6215,7 @@
         <v>0.1741844147037204</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -6219,7 +6226,7 @@
         <v>7.9007782962686582E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -6230,7 +6237,7 @@
         <v>0.44288657618668342</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -6241,7 +6248,7 @@
         <v>0.37982964972805122</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -6252,7 +6259,7 @@
         <v>4.4591654910338729E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -6263,7 +6270,7 @@
         <v>2.5700240496800562E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -6274,7 +6281,7 @@
         <v>0.13019562378812793</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -6291,16 +6298,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -6323,16 +6330,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -6400,7 +6407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6468,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6536,7 +6543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6604,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6672,7 +6679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6740,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -6808,7 +6815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -6876,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -6944,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -7012,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -7080,7 +7087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -7148,7 +7155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -7216,7 +7223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -7284,7 +7291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -7352,7 +7359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -7420,7 +7427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -7488,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -7556,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -7624,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -7692,7 +7699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -7760,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>

</xml_diff>